<commit_message>
Actualizada grafica burn up
</commit_message>
<xml_diff>
--- a/Progreso/BurnUp.xlsx
+++ b/Progreso/BurnUp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\VM\D12-Acme-Pet\Progreso\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\vm\2o cuatrimestre\D12-Acme-Pet\Progreso\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
   <si>
     <t>Revisión 1</t>
   </si>
@@ -494,6 +494,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1721,7 +1724,7 @@
   <dimension ref="A4:F54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1782,6 +1785,10 @@
       <c r="C8" t="s">
         <v>2</v>
       </c>
+      <c r="D8">
+        <f>COUNTIF(E16:E54,"=3")+D7</f>
+        <v>16</v>
+      </c>
       <c r="E8">
         <f>COUNTIF(F16:F54,"=3")+E7</f>
         <v>16</v>
@@ -1956,8 +1963,8 @@
       <c r="D24">
         <v>3</v>
       </c>
-      <c r="E24" t="s">
-        <v>23</v>
+      <c r="E24">
+        <v>3</v>
       </c>
       <c r="F24">
         <v>3</v>
@@ -2012,8 +2019,8 @@
       <c r="D28">
         <v>3</v>
       </c>
-      <c r="E28" t="s">
-        <v>23</v>
+      <c r="E28">
+        <v>3</v>
       </c>
       <c r="F28">
         <v>3</v>
@@ -2026,8 +2033,8 @@
       <c r="D29">
         <v>3</v>
       </c>
-      <c r="E29" t="s">
-        <v>23</v>
+      <c r="E29">
+        <v>3</v>
       </c>
       <c r="F29">
         <v>3</v>
@@ -2040,8 +2047,8 @@
       <c r="D30">
         <v>3</v>
       </c>
-      <c r="E30" t="s">
-        <v>23</v>
+      <c r="E30">
+        <v>3</v>
       </c>
       <c r="F30">
         <v>3</v>
@@ -2054,8 +2061,8 @@
       <c r="D31">
         <v>3</v>
       </c>
-      <c r="E31" t="s">
-        <v>23</v>
+      <c r="E31">
+        <v>3</v>
       </c>
       <c r="F31">
         <v>3</v>
@@ -2166,8 +2173,8 @@
       <c r="D39">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>23</v>
+      <c r="E39">
+        <v>3</v>
       </c>
       <c r="F39">
         <v>4</v>

</xml_diff>

<commit_message>
Actualizado TODO y copiados a words un par de casos de uso mas
</commit_message>
<xml_diff>
--- a/Progreso/BurnUp.xlsx
+++ b/Progreso/BurnUp.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17927"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\vm\2o cuatrimestre\D12-Acme-Pet\Progreso\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Hoja1" sheetId="4" r:id="rId1"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
   <si>
     <t>Revisión 1</t>
   </si>
@@ -187,12 +182,36 @@
   </si>
   <si>
     <t>Redaccion test aceptacion</t>
+  </si>
+  <si>
+    <t>Roldan</t>
+  </si>
+  <si>
+    <t>Acha</t>
+  </si>
+  <si>
+    <t>Javi</t>
+  </si>
+  <si>
+    <t>Roldan, Gavira</t>
+  </si>
+  <si>
+    <t>Dani, Javi</t>
+  </si>
+  <si>
+    <t>Arturo</t>
+  </si>
+  <si>
+    <t>Acha, Roldan</t>
+  </si>
+  <si>
+    <t>Todos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -218,12 +237,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,7 +272,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -289,9 +319,6 @@
           </c:marker>
           <c:dPt>
             <c:idx val="1"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:ln w="114300" cap="rnd">
@@ -302,7 +329,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-1747-40B2-AE14-CE2DBD08F13A}"/>
               </c:ext>
@@ -310,9 +337,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:ln w="114300" cap="rnd">
@@ -323,7 +347,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-1747-40B2-AE14-CE2DBD08F13A}"/>
               </c:ext>
@@ -331,9 +355,6 @@
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
-            <c:marker>
-              <c:symbol val="none"/>
-            </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:ln w="114300" cap="rnd" cmpd="sng">
@@ -344,7 +365,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-1747-40B2-AE14-CE2DBD08F13A}"/>
               </c:ext>
@@ -416,7 +437,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000007-1747-40B2-AE14-CE2DBD08F13A}"/>
             </c:ext>
@@ -498,11 +519,14 @@
                 <c:pt idx="3">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>24</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1747-40B2-AE14-CE2DBD08F13A}"/>
             </c:ext>
@@ -516,12 +540,13 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="549121872"/>
-        <c:axId val="553455216"/>
+        <c:axId val="140233216"/>
+        <c:axId val="152616960"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="549121872"/>
+        <c:axId val="140233216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -553,6 +578,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -561,26 +587,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="4400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -619,7 +625,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="553455216"/>
+        <c:crossAx val="152616960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -627,7 +633,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553455216"/>
+        <c:axId val="152616960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -673,6 +679,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -681,26 +688,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="4400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="es-ES"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -733,7 +720,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="549121872"/>
+        <c:crossAx val="140233216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -747,6 +734,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -813,559 +801,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent5"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1386,7 +821,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{958BCEC4-EB27-4421-99F4-0D9EB3ADA575}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{958BCEC4-EB27-4421-99F4-0D9EB3ADA575}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1452,7 +887,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1504,7 +939,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1698,7 +1133,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1708,23 +1143,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D4" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="AC41" sqref="AC41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:F54"/>
+  <dimension ref="A4:G54"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1798,6 +1234,10 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
+      <c r="D9">
+        <f>COUNTIF(E16:E54,"=4")+D8</f>
+        <v>24</v>
+      </c>
       <c r="E9">
         <f>COUNTIF(F16:F54,"=4")+E8</f>
         <v>27</v>
@@ -2005,8 +1445,8 @@
       <c r="D27">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
-        <v>23</v>
+      <c r="E27">
+        <v>4</v>
       </c>
       <c r="F27">
         <v>3</v>
@@ -2075,14 +1515,14 @@
       <c r="D32">
         <v>4</v>
       </c>
-      <c r="E32" t="s">
-        <v>23</v>
+      <c r="E32">
+        <v>4</v>
       </c>
       <c r="F32">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2095,78 +1535,81 @@
       <c r="F33">
         <v>4</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="D34">
         <v>4</v>
       </c>
-      <c r="E34" t="s">
-        <v>23</v>
+      <c r="E34">
+        <v>4</v>
       </c>
       <c r="F34">
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="D35">
         <v>4</v>
       </c>
-      <c r="E35" t="s">
-        <v>23</v>
+      <c r="E35">
+        <v>4</v>
       </c>
       <c r="F35">
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="D36">
         <v>4</v>
       </c>
-      <c r="E36" t="s">
-        <v>23</v>
+      <c r="E36">
+        <v>4</v>
       </c>
       <c r="F36">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="D37">
         <v>4</v>
       </c>
-      <c r="E37" t="s">
-        <v>23</v>
+      <c r="E37">
+        <v>4</v>
       </c>
       <c r="F37">
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="D38">
         <v>4</v>
       </c>
-      <c r="E38" t="s">
-        <v>23</v>
+      <c r="E38">
+        <v>4</v>
       </c>
       <c r="F38">
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2180,21 +1623,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="D40">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
-        <v>23</v>
+      <c r="E40">
+        <v>4</v>
       </c>
       <c r="F40">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2207,8 +1650,11 @@
       <c r="F41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2221,16 +1667,28 @@
       <c r="F42">
         <v>5</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="G42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F43">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F43" s="1">
+        <v>4</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2243,8 +1701,11 @@
       <c r="F44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2257,8 +1718,11 @@
       <c r="F45">
         <v>6</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -2271,8 +1735,11 @@
       <c r="F46">
         <v>6</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2286,7 +1753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2300,7 +1767,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2313,8 +1780,11 @@
       <c r="F49">
         <v>6</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2327,8 +1797,11 @@
       <c r="F50">
         <v>6</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2341,8 +1814,11 @@
       <c r="F51">
         <v>6</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2355,8 +1831,11 @@
       <c r="F52">
         <v>7</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2370,7 +1849,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>

</xml_diff>